<commit_message>
Pre-CPT version with internal review edits
</commit_message>
<xml_diff>
--- a/examples/smbkc_17/data/VAST vs Design Based.xlsx
+++ b/examples/smbkc_17/data/VAST vs Design Based.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vast DB (2)" sheetId="3" r:id="rId1"/>
@@ -1249,6 +1249,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3905,8 +3906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="240" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="240" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5795,6 +5796,14 @@
         <f t="shared" si="3"/>
         <v>905.72195360453202</v>
       </c>
+      <c r="E33" s="4">
+        <f>AVERAGE(C33:$C$41)/$C$43</f>
+        <v>1.0418962542908687</v>
+      </c>
+      <c r="F33" s="4">
+        <f>C33/$C$43</f>
+        <v>1.0934829616968897</v>
+      </c>
       <c r="G33" s="1">
         <v>0.25600000000000001</v>
       </c>
@@ -5857,6 +5866,14 @@
         <f t="shared" si="3"/>
         <v>1132.7153929460701</v>
       </c>
+      <c r="E34" s="4">
+        <f>AVERAGE(C34:$C$41)/$C$43</f>
+        <v>1.0354479158651162</v>
+      </c>
+      <c r="F34" s="4">
+        <f>C34/$C$43</f>
+        <v>1.9315250745280046</v>
+      </c>
       <c r="G34" s="1">
         <v>0.46600000000000003</v>
       </c>
@@ -5923,7 +5940,10 @@
         <f>AVERAGE(C35:$C$41)/$C$43</f>
         <v>0.90743689319898946</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="4">
+        <f>C35/$C$43</f>
+        <v>1.8968773861266999</v>
+      </c>
       <c r="G35" s="1">
         <v>0.55800000000000005</v>
       </c>
@@ -5990,7 +6010,10 @@
         <f>AVERAGE(C36:$C$41)/$C$43</f>
         <v>0.74253014437770437</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="4">
+        <f>C36/$C$43</f>
+        <v>1.0759130544602018</v>
+      </c>
       <c r="G36" s="1">
         <v>0.33900000000000002</v>
       </c>
@@ -6057,7 +6080,10 @@
         <f>AVERAGE(C37:$C$41)/$C$43</f>
         <v>0.67585356236120486</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="4">
+        <f>C37/$C$43</f>
+        <v>0.39695572674478363</v>
+      </c>
       <c r="G37" s="1">
         <v>0.217</v>
       </c>
@@ -6124,7 +6150,10 @@
         <f>AVERAGE(C38:$C$41)/$C$43</f>
         <v>0.74557802126531014</v>
       </c>
-      <c r="F38" s="4"/>
+      <c r="F38" s="4">
+        <f>C38/$C$43</f>
+        <v>1.046239899947492</v>
+      </c>
       <c r="G38" s="1">
         <v>0.44900000000000001</v>
       </c>
@@ -6191,7 +6220,10 @@
         <f>AVERAGE(C39:$C$41)/$C$43</f>
         <v>0.64535739503791634</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="4">
+        <f>C39/$C$43</f>
+        <v>1.019900569869417</v>
+      </c>
       <c r="G39" s="1">
         <v>0.77</v>
       </c>
@@ -6258,7 +6290,10 @@
         <f>AVERAGE(C40:$C$41)/$C$43</f>
         <v>0.45808580762216589</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="4">
+        <f>C40/$C$43</f>
+        <v>0.60490363320397356</v>
+      </c>
       <c r="G40" s="1">
         <v>0.39300000000000002</v>
       </c>
@@ -6325,7 +6360,10 @@
         <f>AVERAGE(C41:$C$41)/$C$43</f>
         <v>0.31126798204035816</v>
       </c>
-      <c r="F41" s="4"/>
+      <c r="F41" s="4">
+        <f>C41/$C$43</f>
+        <v>0.31126798204035816</v>
+      </c>
       <c r="G41" s="1">
         <v>0.59952907062746896</v>
       </c>

</xml_diff>